<commit_message>
Restricciones y nuevo escenario
</commit_message>
<xml_diff>
--- a/parametros.xlsx
+++ b/parametros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcsalgado\Documents\Adid\tec\tec6\Opti\Reto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EEFA94-E162-4171-B504-5C4D113E8AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF974D4A-E95B-4CEC-A804-53F18A0D2085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3CFAEDAC-BFB0-4A86-949C-30DC1871F13A}"/>
+    <workbookView xWindow="0" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{3CFAEDAC-BFB0-4A86-949C-30DC1871F13A}"/>
   </bookViews>
   <sheets>
     <sheet name="parametros" sheetId="1" r:id="rId1"/>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5389CD99-27DF-4C8A-BD9C-AB30E01D40FD}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +543,7 @@
         <v>31</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>